<commit_message>
UN CAMBIO EN LA SOLICITUD
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado09/guion04/SolicitudGraficaLE_09_04_REC240.xlsx
+++ b/fuentes/contenidos/grado09/guion04/SolicitudGraficaLE_09_04_REC240.xlsx
@@ -638,9 +638,6 @@
     <t>Puño Rojo</t>
   </si>
   <si>
-    <t>Por favor modificar para que diga "Revolución" en la parte inferior. Ubicar en la ficha 1 del ítem "Rojo"</t>
-  </si>
-  <si>
     <t>Niño lanzado una paloma blanca</t>
   </si>
   <si>
@@ -675,6 +672,9 @@
   </si>
   <si>
     <t>Serpiente verde</t>
+  </si>
+  <si>
+    <t>FAVOR CAMBIAR EL TEXTO EN INGLÉS DE ABAJO PARA QUE DIGA: Revolución Ubicar en la ficha 1 del ítem "Rojo"</t>
   </si>
 </sst>
 </file>
@@ -2442,9 +2442,9 @@
   <sheetPr codeName="Hoja1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:P108"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="J1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
+      <selection pane="bottomLeft" activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -2466,7 +2466,7 @@
     <col min="16" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="16.5" thickBot="1">
+    <row r="1" spans="1:16" ht="16" thickBot="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -2485,7 +2485,7 @@
         <v>Ubicación de la imagen en el recurso F6</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="15.75">
+    <row r="2" spans="1:16" ht="15">
       <c r="A2" s="1"/>
       <c r="B2" s="3" t="s">
         <v>121</v>
@@ -2516,7 +2516,7 @@
         <v>M3A</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="15.75">
+    <row r="3" spans="1:16" ht="15">
       <c r="A3" s="1"/>
       <c r="B3" s="4" t="s">
         <v>8</v>
@@ -2547,7 +2547,7 @@
         <v>M5A</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="16.5">
+    <row r="4" spans="1:16" ht="15">
       <c r="A4" s="1"/>
       <c r="B4" s="4" t="s">
         <v>54</v>
@@ -2579,7 +2579,7 @@
         <v>M6A</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="17.25" thickBot="1">
+    <row r="5" spans="1:16" ht="16" thickBot="1">
       <c r="A5" s="1"/>
       <c r="B5" s="6" t="s">
         <v>1</v>
@@ -2612,7 +2612,7 @@
         <v>M7A</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="16.5" thickBot="1">
+    <row r="6" spans="1:16" ht="16" thickBot="1">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -2665,7 +2665,7 @@
         <v>M9B</v>
       </c>
     </row>
-    <row r="8" spans="1:16" s="8" customFormat="1" ht="16.5" thickBot="1">
+    <row r="8" spans="1:16" s="8" customFormat="1" ht="16" thickBot="1">
       <c r="A8" s="9"/>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
@@ -2777,7 +2777,7 @@
         <v>M12D</v>
       </c>
     </row>
-    <row r="11" spans="1:16" s="11" customFormat="1" ht="39">
+    <row r="11" spans="1:16" s="11" customFormat="1" ht="52">
       <c r="A11" s="12" t="str">
         <f>IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE(LEFT(A10,3),IF(MID(A10,4,2)+1&lt;10,CONCATENATE("0",MID(A10,4,2)+1))),"")</f>
         <v>IMG02</v>
@@ -2815,7 +2815,7 @@
         <v>202</v>
       </c>
       <c r="K11" s="65" t="s">
-        <v>203</v>
+        <v>215</v>
       </c>
       <c r="O11" s="2" t="str">
         <f>'Definición técnica de imagenes'!A13</f>
@@ -2992,7 +2992,7 @@
         <v/>
       </c>
       <c r="J15" s="66" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="K15" s="64" t="s">
         <v>200</v>
@@ -3037,7 +3037,7 @@
         <v/>
       </c>
       <c r="J16" s="67" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="K16" s="64" t="s">
         <v>201</v>
@@ -3082,10 +3082,10 @@
         <v>800 x 458 px</v>
       </c>
       <c r="J17" s="66" t="s">
+        <v>203</v>
+      </c>
+      <c r="K17" s="66" t="s">
         <v>204</v>
-      </c>
-      <c r="K17" s="66" t="s">
-        <v>205</v>
       </c>
       <c r="O17" s="2" t="str">
         <f>'Definición técnica de imagenes'!A27</f>
@@ -3127,10 +3127,10 @@
         <v>800 x 458 px</v>
       </c>
       <c r="J18" s="66" t="s">
+        <v>205</v>
+      </c>
+      <c r="K18" s="66" t="s">
         <v>206</v>
-      </c>
-      <c r="K18" s="66" t="s">
-        <v>207</v>
       </c>
       <c r="O18" s="2" t="str">
         <f>'Definición técnica de imagenes'!A30</f>
@@ -3172,10 +3172,10 @@
         <v>800 x 458 px</v>
       </c>
       <c r="J19" s="67" t="s">
+        <v>208</v>
+      </c>
+      <c r="K19" s="66" t="s">
         <v>209</v>
-      </c>
-      <c r="K19" s="66" t="s">
-        <v>210</v>
       </c>
       <c r="O19" s="2" t="str">
         <f>'Definición técnica de imagenes'!A31</f>
@@ -3217,10 +3217,10 @@
         <v>800 x 458 px</v>
       </c>
       <c r="J20" s="64" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="K20" s="66" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="O20" s="2" t="str">
         <f>'Definición técnica de imagenes'!A32</f>
@@ -3262,17 +3262,17 @@
         <v>800 x 458 px</v>
       </c>
       <c r="J21" s="66" t="s">
+        <v>212</v>
+      </c>
+      <c r="K21" s="66" t="s">
         <v>213</v>
-      </c>
-      <c r="K21" s="66" t="s">
-        <v>214</v>
       </c>
       <c r="O21" s="2" t="str">
         <f>'Definición técnica de imagenes'!A33</f>
         <v>F11</v>
       </c>
     </row>
-    <row r="22" spans="1:15" s="11" customFormat="1" ht="15">
+    <row r="22" spans="1:15" s="11" customFormat="1">
       <c r="A22" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3307,7 +3307,7 @@
         <v>F12</v>
       </c>
     </row>
-    <row r="23" spans="1:15" s="11" customFormat="1" ht="15">
+    <row r="23" spans="1:15" s="11" customFormat="1">
       <c r="A23" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3342,7 +3342,7 @@
         <v>F13</v>
       </c>
     </row>
-    <row r="24" spans="1:15" s="11" customFormat="1" ht="15">
+    <row r="24" spans="1:15" s="11" customFormat="1">
       <c r="A24" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3377,7 +3377,7 @@
         <v>F13B</v>
       </c>
     </row>
-    <row r="25" spans="1:15" s="11" customFormat="1" ht="15">
+    <row r="25" spans="1:15" s="11" customFormat="1">
       <c r="A25" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3408,7 +3408,7 @@
       <c r="J25" s="63"/>
       <c r="K25" s="64"/>
     </row>
-    <row r="26" spans="1:15" s="11" customFormat="1" ht="15">
+    <row r="26" spans="1:15" s="11" customFormat="1">
       <c r="A26" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3439,7 +3439,7 @@
       <c r="J26" s="63"/>
       <c r="K26" s="64"/>
     </row>
-    <row r="27" spans="1:15" s="11" customFormat="1" ht="15">
+    <row r="27" spans="1:15" s="11" customFormat="1">
       <c r="A27" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3471,7 +3471,7 @@
       <c r="K27" s="64"/>
       <c r="O27" s="2"/>
     </row>
-    <row r="28" spans="1:15" s="11" customFormat="1" ht="15">
+    <row r="28" spans="1:15" s="11" customFormat="1">
       <c r="A28" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3502,7 +3502,7 @@
       <c r="J28" s="64"/>
       <c r="K28" s="64"/>
     </row>
-    <row r="29" spans="1:15" s="11" customFormat="1" ht="15">
+    <row r="29" spans="1:15" s="11" customFormat="1">
       <c r="A29" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3533,7 +3533,7 @@
       <c r="J29" s="64"/>
       <c r="K29" s="64"/>
     </row>
-    <row r="30" spans="1:15" s="11" customFormat="1" ht="15">
+    <row r="30" spans="1:15" s="11" customFormat="1">
       <c r="A30" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3564,7 +3564,7 @@
       <c r="J30" s="64"/>
       <c r="K30" s="64"/>
     </row>
-    <row r="31" spans="1:15" s="11" customFormat="1" ht="15">
+    <row r="31" spans="1:15" s="11" customFormat="1">
       <c r="A31" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3595,7 +3595,7 @@
       <c r="J31" s="64"/>
       <c r="K31" s="64"/>
     </row>
-    <row r="32" spans="1:15" s="11" customFormat="1" ht="15">
+    <row r="32" spans="1:15" s="11" customFormat="1">
       <c r="A32" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3626,7 +3626,7 @@
       <c r="J32" s="64"/>
       <c r="K32" s="64"/>
     </row>
-    <row r="33" spans="1:15" s="11" customFormat="1" ht="15">
+    <row r="33" spans="1:15" s="11" customFormat="1">
       <c r="A33" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3657,7 +3657,7 @@
       <c r="J33" s="64"/>
       <c r="K33" s="64"/>
     </row>
-    <row r="34" spans="1:15" s="11" customFormat="1" ht="15">
+    <row r="34" spans="1:15" s="11" customFormat="1">
       <c r="A34" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3689,7 +3689,7 @@
       <c r="K34" s="64"/>
       <c r="O34" s="2"/>
     </row>
-    <row r="35" spans="1:15" s="11" customFormat="1" ht="15">
+    <row r="35" spans="1:15" s="11" customFormat="1">
       <c r="A35" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3721,7 +3721,7 @@
       <c r="K35" s="65"/>
       <c r="O35" s="2"/>
     </row>
-    <row r="36" spans="1:15" s="11" customFormat="1" ht="15">
+    <row r="36" spans="1:15" s="11" customFormat="1">
       <c r="A36" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3753,7 +3753,7 @@
       <c r="K36" s="65"/>
       <c r="O36" s="2"/>
     </row>
-    <row r="37" spans="1:15" s="11" customFormat="1" ht="15">
+    <row r="37" spans="1:15" s="11" customFormat="1">
       <c r="A37" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3784,7 +3784,7 @@
       <c r="J37" s="69"/>
       <c r="K37" s="65"/>
     </row>
-    <row r="38" spans="1:15" s="11" customFormat="1" ht="15">
+    <row r="38" spans="1:15" s="11" customFormat="1">
       <c r="A38" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3815,7 +3815,7 @@
       <c r="J38" s="70"/>
       <c r="K38" s="65"/>
     </row>
-    <row r="39" spans="1:15" s="11" customFormat="1" ht="15">
+    <row r="39" spans="1:15" s="11" customFormat="1">
       <c r="A39" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3846,7 +3846,7 @@
       <c r="J39" s="63"/>
       <c r="K39" s="65"/>
     </row>
-    <row r="40" spans="1:15" s="11" customFormat="1" ht="15">
+    <row r="40" spans="1:15" s="11" customFormat="1">
       <c r="A40" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3877,7 +3877,7 @@
       <c r="J40" s="63"/>
       <c r="K40" s="65"/>
     </row>
-    <row r="41" spans="1:15" s="11" customFormat="1" ht="15">
+    <row r="41" spans="1:15" s="11" customFormat="1">
       <c r="A41" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3908,7 +3908,7 @@
       <c r="J41" s="63"/>
       <c r="K41" s="65"/>
     </row>
-    <row r="42" spans="1:15" s="11" customFormat="1" ht="15">
+    <row r="42" spans="1:15" s="11" customFormat="1">
       <c r="A42" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3939,7 +3939,7 @@
       <c r="J42" s="63"/>
       <c r="K42" s="65"/>
     </row>
-    <row r="43" spans="1:15" s="11" customFormat="1" ht="15">
+    <row r="43" spans="1:15" s="11" customFormat="1">
       <c r="A43" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3970,7 +3970,7 @@
       <c r="J43" s="63"/>
       <c r="K43" s="65"/>
     </row>
-    <row r="44" spans="1:15" s="11" customFormat="1" ht="15">
+    <row r="44" spans="1:15" s="11" customFormat="1">
       <c r="A44" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4001,7 +4001,7 @@
       <c r="J44" s="63"/>
       <c r="K44" s="65"/>
     </row>
-    <row r="45" spans="1:15" s="11" customFormat="1" ht="15">
+    <row r="45" spans="1:15" s="11" customFormat="1">
       <c r="A45" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4032,7 +4032,7 @@
       <c r="J45" s="63"/>
       <c r="K45" s="65"/>
     </row>
-    <row r="46" spans="1:15" s="11" customFormat="1" ht="15">
+    <row r="46" spans="1:15" s="11" customFormat="1">
       <c r="A46" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4063,7 +4063,7 @@
       <c r="J46" s="63"/>
       <c r="K46" s="65"/>
     </row>
-    <row r="47" spans="1:15" s="11" customFormat="1" ht="15">
+    <row r="47" spans="1:15" s="11" customFormat="1">
       <c r="A47" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4094,7 +4094,7 @@
       <c r="J47" s="63"/>
       <c r="K47" s="65"/>
     </row>
-    <row r="48" spans="1:15" s="11" customFormat="1" ht="15">
+    <row r="48" spans="1:15" s="11" customFormat="1">
       <c r="A48" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4125,7 +4125,7 @@
       <c r="J48" s="63"/>
       <c r="K48" s="65"/>
     </row>
-    <row r="49" spans="1:11" s="11" customFormat="1" ht="15">
+    <row r="49" spans="1:11" s="11" customFormat="1">
       <c r="A49" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4156,7 +4156,7 @@
       <c r="J49" s="63"/>
       <c r="K49" s="65"/>
     </row>
-    <row r="50" spans="1:11" s="11" customFormat="1" ht="15">
+    <row r="50" spans="1:11" s="11" customFormat="1">
       <c r="A50" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4187,7 +4187,7 @@
       <c r="J50" s="63"/>
       <c r="K50" s="65"/>
     </row>
-    <row r="51" spans="1:11" s="11" customFormat="1" ht="15">
+    <row r="51" spans="1:11" s="11" customFormat="1">
       <c r="A51" s="12" t="str">
         <f t="shared" ref="A51:A82" si="8">IF(OR(B51&lt;&gt;"",J51&lt;&gt;""),CONCATENATE(LEFT(A50,3),IF(MID(A50,4,2)+1&lt;10,CONCATENATE("0",MID(A50,4,2)+1),MID(A50,4,2)+1)),"")</f>
         <v/>
@@ -4218,7 +4218,7 @@
       <c r="J51" s="63"/>
       <c r="K51" s="65"/>
     </row>
-    <row r="52" spans="1:11" s="11" customFormat="1" ht="15">
+    <row r="52" spans="1:11" s="11" customFormat="1">
       <c r="A52" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4249,7 +4249,7 @@
       <c r="J52" s="63"/>
       <c r="K52" s="65"/>
     </row>
-    <row r="53" spans="1:11" s="11" customFormat="1" ht="15">
+    <row r="53" spans="1:11" s="11" customFormat="1">
       <c r="A53" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4280,7 +4280,7 @@
       <c r="J53" s="63"/>
       <c r="K53" s="65"/>
     </row>
-    <row r="54" spans="1:11" s="11" customFormat="1" ht="15">
+    <row r="54" spans="1:11" s="11" customFormat="1">
       <c r="A54" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4311,7 +4311,7 @@
       <c r="J54" s="63"/>
       <c r="K54" s="65"/>
     </row>
-    <row r="55" spans="1:11" s="11" customFormat="1" ht="15">
+    <row r="55" spans="1:11" s="11" customFormat="1">
       <c r="A55" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4342,7 +4342,7 @@
       <c r="J55" s="63"/>
       <c r="K55" s="65"/>
     </row>
-    <row r="56" spans="1:11" s="11" customFormat="1" ht="15">
+    <row r="56" spans="1:11" s="11" customFormat="1">
       <c r="A56" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4373,7 +4373,7 @@
       <c r="J56" s="63"/>
       <c r="K56" s="65"/>
     </row>
-    <row r="57" spans="1:11" s="11" customFormat="1" ht="15">
+    <row r="57" spans="1:11" s="11" customFormat="1">
       <c r="A57" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4404,7 +4404,7 @@
       <c r="J57" s="63"/>
       <c r="K57" s="65"/>
     </row>
-    <row r="58" spans="1:11" s="11" customFormat="1" ht="15">
+    <row r="58" spans="1:11" s="11" customFormat="1">
       <c r="A58" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4435,7 +4435,7 @@
       <c r="J58" s="63"/>
       <c r="K58" s="65"/>
     </row>
-    <row r="59" spans="1:11" s="11" customFormat="1" ht="15">
+    <row r="59" spans="1:11" s="11" customFormat="1">
       <c r="A59" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4466,7 +4466,7 @@
       <c r="J59" s="63"/>
       <c r="K59" s="65"/>
     </row>
-    <row r="60" spans="1:11" s="11" customFormat="1" ht="15">
+    <row r="60" spans="1:11" s="11" customFormat="1">
       <c r="A60" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4497,7 +4497,7 @@
       <c r="J60" s="63"/>
       <c r="K60" s="65"/>
     </row>
-    <row r="61" spans="1:11" s="11" customFormat="1" ht="15">
+    <row r="61" spans="1:11" s="11" customFormat="1">
       <c r="A61" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4528,7 +4528,7 @@
       <c r="J61" s="63"/>
       <c r="K61" s="65"/>
     </row>
-    <row r="62" spans="1:11" s="11" customFormat="1" ht="15">
+    <row r="62" spans="1:11" s="11" customFormat="1">
       <c r="A62" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4559,7 +4559,7 @@
       <c r="J62" s="63"/>
       <c r="K62" s="65"/>
     </row>
-    <row r="63" spans="1:11" s="11" customFormat="1" ht="15">
+    <row r="63" spans="1:11" s="11" customFormat="1">
       <c r="A63" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4590,7 +4590,7 @@
       <c r="J63" s="63"/>
       <c r="K63" s="65"/>
     </row>
-    <row r="64" spans="1:11" s="11" customFormat="1" ht="15">
+    <row r="64" spans="1:11" s="11" customFormat="1">
       <c r="A64" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4621,7 +4621,7 @@
       <c r="J64" s="63"/>
       <c r="K64" s="65"/>
     </row>
-    <row r="65" spans="1:11" s="11" customFormat="1" ht="15">
+    <row r="65" spans="1:11" s="11" customFormat="1">
       <c r="A65" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4652,7 +4652,7 @@
       <c r="J65" s="63"/>
       <c r="K65" s="65"/>
     </row>
-    <row r="66" spans="1:11" s="11" customFormat="1" ht="15">
+    <row r="66" spans="1:11" s="11" customFormat="1">
       <c r="A66" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4683,7 +4683,7 @@
       <c r="J66" s="63"/>
       <c r="K66" s="65"/>
     </row>
-    <row r="67" spans="1:11" s="11" customFormat="1" ht="15">
+    <row r="67" spans="1:11" s="11" customFormat="1">
       <c r="A67" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4714,7 +4714,7 @@
       <c r="J67" s="63"/>
       <c r="K67" s="65"/>
     </row>
-    <row r="68" spans="1:11" s="11" customFormat="1" ht="15">
+    <row r="68" spans="1:11" s="11" customFormat="1">
       <c r="A68" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4745,7 +4745,7 @@
       <c r="J68" s="63"/>
       <c r="K68" s="65"/>
     </row>
-    <row r="69" spans="1:11" s="11" customFormat="1" ht="15">
+    <row r="69" spans="1:11" s="11" customFormat="1">
       <c r="A69" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4776,7 +4776,7 @@
       <c r="J69" s="63"/>
       <c r="K69" s="65"/>
     </row>
-    <row r="70" spans="1:11" s="11" customFormat="1" ht="15">
+    <row r="70" spans="1:11" s="11" customFormat="1">
       <c r="A70" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4807,7 +4807,7 @@
       <c r="J70" s="63"/>
       <c r="K70" s="65"/>
     </row>
-    <row r="71" spans="1:11" s="11" customFormat="1" ht="15">
+    <row r="71" spans="1:11" s="11" customFormat="1">
       <c r="A71" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4838,7 +4838,7 @@
       <c r="J71" s="63"/>
       <c r="K71" s="65"/>
     </row>
-    <row r="72" spans="1:11" s="11" customFormat="1" ht="15">
+    <row r="72" spans="1:11" s="11" customFormat="1">
       <c r="A72" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4869,7 +4869,7 @@
       <c r="J72" s="63"/>
       <c r="K72" s="65"/>
     </row>
-    <row r="73" spans="1:11" s="11" customFormat="1" ht="15">
+    <row r="73" spans="1:11" s="11" customFormat="1">
       <c r="A73" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4900,7 +4900,7 @@
       <c r="J73" s="63"/>
       <c r="K73" s="65"/>
     </row>
-    <row r="74" spans="1:11" s="11" customFormat="1" ht="15">
+    <row r="74" spans="1:11" s="11" customFormat="1">
       <c r="A74" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4931,7 +4931,7 @@
       <c r="J74" s="63"/>
       <c r="K74" s="65"/>
     </row>
-    <row r="75" spans="1:11" s="11" customFormat="1" ht="15">
+    <row r="75" spans="1:11" s="11" customFormat="1">
       <c r="A75" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4962,7 +4962,7 @@
       <c r="J75" s="63"/>
       <c r="K75" s="65"/>
     </row>
-    <row r="76" spans="1:11" s="11" customFormat="1" ht="15">
+    <row r="76" spans="1:11" s="11" customFormat="1">
       <c r="A76" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4993,7 +4993,7 @@
       <c r="J76" s="63"/>
       <c r="K76" s="65"/>
     </row>
-    <row r="77" spans="1:11" s="11" customFormat="1" ht="15">
+    <row r="77" spans="1:11" s="11" customFormat="1">
       <c r="A77" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5024,7 +5024,7 @@
       <c r="J77" s="63"/>
       <c r="K77" s="65"/>
     </row>
-    <row r="78" spans="1:11" s="11" customFormat="1" ht="15">
+    <row r="78" spans="1:11" s="11" customFormat="1">
       <c r="A78" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5055,7 +5055,7 @@
       <c r="J78" s="63"/>
       <c r="K78" s="65"/>
     </row>
-    <row r="79" spans="1:11" s="11" customFormat="1" ht="15">
+    <row r="79" spans="1:11" s="11" customFormat="1">
       <c r="A79" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5086,7 +5086,7 @@
       <c r="J79" s="63"/>
       <c r="K79" s="65"/>
     </row>
-    <row r="80" spans="1:11" s="11" customFormat="1" ht="15">
+    <row r="80" spans="1:11" s="11" customFormat="1">
       <c r="A80" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5117,7 +5117,7 @@
       <c r="J80" s="63"/>
       <c r="K80" s="65"/>
     </row>
-    <row r="81" spans="1:11" s="11" customFormat="1" ht="15">
+    <row r="81" spans="1:11" s="11" customFormat="1">
       <c r="A81" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5148,7 +5148,7 @@
       <c r="J81" s="63"/>
       <c r="K81" s="65"/>
     </row>
-    <row r="82" spans="1:11" s="11" customFormat="1" ht="15">
+    <row r="82" spans="1:11" s="11" customFormat="1">
       <c r="A82" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5179,7 +5179,7 @@
       <c r="J82" s="63"/>
       <c r="K82" s="65"/>
     </row>
-    <row r="83" spans="1:11" s="11" customFormat="1" ht="15">
+    <row r="83" spans="1:11" s="11" customFormat="1">
       <c r="A83" s="12" t="str">
         <f t="shared" ref="A83:A108" si="12">IF(OR(B83&lt;&gt;"",J83&lt;&gt;""),CONCATENATE(LEFT(A82,3),IF(MID(A82,4,2)+1&lt;10,CONCATENATE("0",MID(A82,4,2)+1),MID(A82,4,2)+1)),"")</f>
         <v/>
@@ -5210,7 +5210,7 @@
       <c r="J83" s="63"/>
       <c r="K83" s="65"/>
     </row>
-    <row r="84" spans="1:11" s="11" customFormat="1" ht="15">
+    <row r="84" spans="1:11" s="11" customFormat="1">
       <c r="A84" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5241,7 +5241,7 @@
       <c r="J84" s="63"/>
       <c r="K84" s="65"/>
     </row>
-    <row r="85" spans="1:11" s="11" customFormat="1" ht="15">
+    <row r="85" spans="1:11" s="11" customFormat="1">
       <c r="A85" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5272,7 +5272,7 @@
       <c r="J85" s="63"/>
       <c r="K85" s="65"/>
     </row>
-    <row r="86" spans="1:11" s="11" customFormat="1" ht="15">
+    <row r="86" spans="1:11" s="11" customFormat="1">
       <c r="A86" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5303,7 +5303,7 @@
       <c r="J86" s="63"/>
       <c r="K86" s="65"/>
     </row>
-    <row r="87" spans="1:11" s="11" customFormat="1" ht="15">
+    <row r="87" spans="1:11" s="11" customFormat="1">
       <c r="A87" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5334,7 +5334,7 @@
       <c r="J87" s="63"/>
       <c r="K87" s="65"/>
     </row>
-    <row r="88" spans="1:11" s="11" customFormat="1" ht="15">
+    <row r="88" spans="1:11" s="11" customFormat="1">
       <c r="A88" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5365,7 +5365,7 @@
       <c r="J88" s="63"/>
       <c r="K88" s="65"/>
     </row>
-    <row r="89" spans="1:11" s="11" customFormat="1" ht="15">
+    <row r="89" spans="1:11" s="11" customFormat="1">
       <c r="A89" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5396,7 +5396,7 @@
       <c r="J89" s="63"/>
       <c r="K89" s="65"/>
     </row>
-    <row r="90" spans="1:11" s="11" customFormat="1" ht="15">
+    <row r="90" spans="1:11" s="11" customFormat="1">
       <c r="A90" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5427,7 +5427,7 @@
       <c r="J90" s="63"/>
       <c r="K90" s="65"/>
     </row>
-    <row r="91" spans="1:11" s="11" customFormat="1" ht="15">
+    <row r="91" spans="1:11" s="11" customFormat="1">
       <c r="A91" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5458,7 +5458,7 @@
       <c r="J91" s="63"/>
       <c r="K91" s="65"/>
     </row>
-    <row r="92" spans="1:11" s="11" customFormat="1" ht="15">
+    <row r="92" spans="1:11" s="11" customFormat="1">
       <c r="A92" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5489,7 +5489,7 @@
       <c r="J92" s="63"/>
       <c r="K92" s="65"/>
     </row>
-    <row r="93" spans="1:11" s="11" customFormat="1" ht="15">
+    <row r="93" spans="1:11" s="11" customFormat="1">
       <c r="A93" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5520,7 +5520,7 @@
       <c r="J93" s="63"/>
       <c r="K93" s="65"/>
     </row>
-    <row r="94" spans="1:11" s="11" customFormat="1" ht="15">
+    <row r="94" spans="1:11" s="11" customFormat="1">
       <c r="A94" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5551,7 +5551,7 @@
       <c r="J94" s="63"/>
       <c r="K94" s="65"/>
     </row>
-    <row r="95" spans="1:11" s="11" customFormat="1" ht="15">
+    <row r="95" spans="1:11" s="11" customFormat="1">
       <c r="A95" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5582,7 +5582,7 @@
       <c r="J95" s="63"/>
       <c r="K95" s="65"/>
     </row>
-    <row r="96" spans="1:11" s="11" customFormat="1" ht="15">
+    <row r="96" spans="1:11" s="11" customFormat="1">
       <c r="A96" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5613,7 +5613,7 @@
       <c r="J96" s="63"/>
       <c r="K96" s="65"/>
     </row>
-    <row r="97" spans="1:11" s="11" customFormat="1" ht="15">
+    <row r="97" spans="1:11" s="11" customFormat="1">
       <c r="A97" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5644,7 +5644,7 @@
       <c r="J97" s="63"/>
       <c r="K97" s="65"/>
     </row>
-    <row r="98" spans="1:11" s="11" customFormat="1" ht="15">
+    <row r="98" spans="1:11" s="11" customFormat="1">
       <c r="A98" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5675,7 +5675,7 @@
       <c r="J98" s="63"/>
       <c r="K98" s="65"/>
     </row>
-    <row r="99" spans="1:11" s="11" customFormat="1" ht="15">
+    <row r="99" spans="1:11" s="11" customFormat="1">
       <c r="A99" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5706,7 +5706,7 @@
       <c r="J99" s="63"/>
       <c r="K99" s="65"/>
     </row>
-    <row r="100" spans="1:11" s="11" customFormat="1" ht="15">
+    <row r="100" spans="1:11" s="11" customFormat="1">
       <c r="A100" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5737,7 +5737,7 @@
       <c r="J100" s="63"/>
       <c r="K100" s="65"/>
     </row>
-    <row r="101" spans="1:11" s="11" customFormat="1" ht="15">
+    <row r="101" spans="1:11" s="11" customFormat="1">
       <c r="A101" s="12" t="str">
         <f>IF(OR(B101&lt;&gt;"",J101&lt;&gt;""),CONCATENATE(LEFT(A100,3),IF(MID(A100,4,2)+1&lt;10,CONCATENATE("0",MID(A100,4,2)+1),MID(A100,4,2)+1)),"")</f>
         <v/>
@@ -5768,7 +5768,7 @@
       <c r="J101" s="63"/>
       <c r="K101" s="65"/>
     </row>
-    <row r="102" spans="1:11" s="11" customFormat="1" ht="15">
+    <row r="102" spans="1:11" s="11" customFormat="1">
       <c r="A102" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5799,7 +5799,7 @@
       <c r="J102" s="63"/>
       <c r="K102" s="65"/>
     </row>
-    <row r="103" spans="1:11" s="11" customFormat="1" ht="15">
+    <row r="103" spans="1:11" s="11" customFormat="1">
       <c r="A103" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5830,7 +5830,7 @@
       <c r="J103" s="63"/>
       <c r="K103" s="65"/>
     </row>
-    <row r="104" spans="1:11" s="11" customFormat="1" ht="15">
+    <row r="104" spans="1:11" s="11" customFormat="1">
       <c r="A104" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5861,7 +5861,7 @@
       <c r="J104" s="63"/>
       <c r="K104" s="65"/>
     </row>
-    <row r="105" spans="1:11" s="11" customFormat="1" ht="15">
+    <row r="105" spans="1:11" s="11" customFormat="1">
       <c r="A105" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5892,7 +5892,7 @@
       <c r="J105" s="63"/>
       <c r="K105" s="65"/>
     </row>
-    <row r="106" spans="1:11" s="11" customFormat="1" ht="15">
+    <row r="106" spans="1:11" s="11" customFormat="1">
       <c r="A106" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5923,7 +5923,7 @@
       <c r="J106" s="63"/>
       <c r="K106" s="65"/>
     </row>
-    <row r="107" spans="1:11" s="11" customFormat="1" ht="15">
+    <row r="107" spans="1:11" s="11" customFormat="1">
       <c r="A107" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5954,7 +5954,7 @@
       <c r="J107" s="63"/>
       <c r="K107" s="65"/>
     </row>
-    <row r="108" spans="1:11" s="11" customFormat="1" ht="15">
+    <row r="108" spans="1:11" s="11" customFormat="1">
       <c r="A108" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -6055,7 +6055,7 @@
     <col min="12" max="16384" width="10.83203125" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="16.5" thickBot="1">
+    <row r="1" spans="1:11" ht="16" thickBot="1">
       <c r="A1" s="92" t="s">
         <v>38</v>
       </c>
@@ -6077,7 +6077,7 @@
       <c r="E2" s="97"/>
       <c r="F2" s="32"/>
     </row>
-    <row r="3" spans="1:11" ht="63">
+    <row r="3" spans="1:11" ht="60">
       <c r="A3" s="33" t="s">
         <v>43</v>
       </c>
@@ -6101,7 +6101,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="31.5">
+    <row r="4" spans="1:11" ht="30">
       <c r="A4" s="30" t="s">
         <v>44</v>
       </c>
@@ -6129,7 +6129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="79.5" thickBot="1">
+    <row r="5" spans="1:11" ht="76" thickBot="1">
       <c r="A5" s="33" t="s">
         <v>45</v>
       </c>
@@ -6156,7 +6156,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="32.25" thickBot="1">
+    <row r="6" spans="1:11" ht="31" thickBot="1">
       <c r="A6" s="30" t="s">
         <v>10</v>
       </c>
@@ -6178,7 +6178,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="48" thickBot="1">
+    <row r="7" spans="1:11" ht="46" thickBot="1">
       <c r="A7" s="33" t="s">
         <v>11</v>
       </c>
@@ -6205,7 +6205,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="47.25">
+    <row r="8" spans="1:11" ht="45">
       <c r="A8" s="33" t="s">
         <v>53</v>
       </c>
@@ -6224,7 +6224,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="47.25">
+    <row r="9" spans="1:11" ht="45">
       <c r="A9" s="33" t="s">
         <v>12</v>
       </c>
@@ -6243,7 +6243,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="32.25" thickBot="1">
+    <row r="10" spans="1:11" ht="31" thickBot="1">
       <c r="A10" s="34" t="s">
         <v>36</v>
       </c>
@@ -6273,7 +6273,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="16.5" thickBot="1">
+    <row r="12" spans="1:11" ht="16" thickBot="1">
       <c r="I12" s="22" t="s">
         <v>37</v>
       </c>
@@ -6303,7 +6303,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="16.5" thickBot="1">
+    <row r="14" spans="1:11" ht="16" thickBot="1">
       <c r="A14" s="33"/>
       <c r="B14" s="31"/>
       <c r="C14" s="31"/>
@@ -6383,7 +6383,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="79.5" thickBot="1">
+    <row r="18" spans="1:11" ht="76" thickBot="1">
       <c r="A18" s="33" t="s">
         <v>48</v>
       </c>
@@ -6423,7 +6423,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="63.75" thickBot="1">
+    <row r="20" spans="1:11" ht="61" thickBot="1">
       <c r="A20" s="34" t="s">
         <v>51</v>
       </c>
@@ -7802,7 +7802,7 @@
       <c r="E43" s="55"/>
       <c r="F43" s="55"/>
     </row>
-    <row r="44" spans="1:9" ht="31.5">
+    <row r="44" spans="1:9" ht="30">
       <c r="A44" s="54" t="s">
         <v>111</v>
       </c>
@@ -7830,7 +7830,7 @@
       <c r="E45" s="55"/>
       <c r="F45" s="55"/>
     </row>
-    <row r="46" spans="1:9" ht="47.25">
+    <row r="46" spans="1:9" ht="45">
       <c r="A46" s="54" t="s">
         <v>162</v>
       </c>

</xml_diff>